<commit_message>
Solicitud_Grafica_Atendida_LE_10_05_REC120 (De la 1 a la 5)
Solicitó editor Luis Felipe.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion05/SolicitudGrafica_LE_10_05_REC120.xlsx
+++ b/fuentes/contenidos/grado10/guion05/SolicitudGrafica_LE_10_05_REC120.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marisolrobayo/Desktop/AULA PLANETA/Lenguaje/fuentes/contenidos/grado10/guion05/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -624,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -785,8 +790,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +845,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -1280,7 +1297,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1338,8 +1355,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1660,8 +1678,11 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="5" xfId="57" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="58">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1718,6 +1739,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Incorrecto" xfId="57" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1815,7 +1837,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1823,6 +1845,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1856,7 +1892,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1864,6 +1900,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1897,7 +1947,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1905,6 +1955,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1938,7 +2002,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1946,6 +2010,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1979,7 +2057,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1987,6 +2065,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2020,7 +2112,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2028,6 +2120,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2061,7 +2167,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2069,6 +2175,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2406,10 +2526,10 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -2428,7 +2548,7 @@
     <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1">
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2447,7 +2567,7 @@
         <v>Ubicación de la imagen en el recurso F4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
@@ -2478,7 +2598,7 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15">
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2507,7 +2627,7 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15">
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2539,7 +2659,7 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16" thickBot="1">
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2572,7 +2692,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16" thickBot="1">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2596,7 +2716,7 @@
         <v>M8A</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
@@ -2625,7 +2745,7 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="16" thickBot="1">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2652,7 +2772,7 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1">
+    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -2692,7 +2812,7 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -2714,7 +2834,7 @@
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_10_05_REC120_IMG01.jpg</v>
       </c>
-      <c r="G10" s="13" t="str">
+      <c r="G10" s="109" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>950 x 435 px</v>
       </c>
@@ -2735,7 +2855,7 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2757,7 +2877,7 @@
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_10_05_REC120_IMG02.jpg</v>
       </c>
-      <c r="G11" s="13" t="str">
+      <c r="G11" s="109" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>330 x 475 px</v>
       </c>
@@ -2778,7 +2898,7 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
@@ -2800,7 +2920,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>LE_10_05_REC120_IMG03.jpg</v>
       </c>
-      <c r="G12" s="13" t="str">
+      <c r="G12" s="109" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>750 x 365 px</v>
       </c>
@@ -2821,7 +2941,7 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
@@ -2843,7 +2963,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>LE_10_05_REC120_IMG04.jpg</v>
       </c>
-      <c r="G13" s="13" t="str">
+      <c r="G13" s="109" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>750 x 365 px</v>
       </c>
@@ -2864,7 +2984,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -2886,7 +3006,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>LE_10_05_REC120_IMG05.jpg</v>
       </c>
-      <c r="G14" s="13" t="str">
+      <c r="G14" s="109" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>750 x 365 px</v>
       </c>
@@ -2907,7 +3027,7 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1">
+    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2942,7 +3062,7 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1">
+    <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2977,7 +3097,7 @@
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1">
+    <row r="17" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3012,7 +3132,7 @@
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1">
+    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3047,7 +3167,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1">
+    <row r="19" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
@@ -3082,7 +3202,7 @@
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1">
+    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3117,7 +3237,7 @@
         <v>F10B</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1">
+    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3152,7 +3272,7 @@
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1">
+    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3187,7 +3307,7 @@
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1">
+    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3222,7 +3342,7 @@
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1">
+    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3257,7 +3377,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1">
+    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3288,7 +3408,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1">
+    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3319,7 +3439,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1">
+    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3351,7 +3471,7 @@
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1">
+    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3382,7 +3502,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1">
+    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3413,7 +3533,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1">
+    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3444,7 +3564,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1">
+    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3475,7 +3595,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1">
+    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3506,7 +3626,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1">
+    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3537,7 +3657,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1">
+    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3569,7 +3689,7 @@
       <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1">
+    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3601,7 +3721,7 @@
       <c r="K35" s="65"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1">
+    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3633,7 +3753,7 @@
       <c r="K36" s="65"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1">
+    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3664,7 +3784,7 @@
       <c r="J37" s="70"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1">
+    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3695,7 +3815,7 @@
       <c r="J38" s="71"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1">
+    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3726,7 +3846,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="11" customFormat="1">
+    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3757,7 +3877,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:15" s="11" customFormat="1">
+    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3788,7 +3908,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1">
+    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3819,7 +3939,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1">
+    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3850,7 +3970,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:15" s="11" customFormat="1">
+    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3881,7 +4001,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1">
+    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3912,7 +4032,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:15" s="11" customFormat="1">
+    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3943,7 +4063,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:15" s="11" customFormat="1">
+    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3974,7 +4094,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:15" s="11" customFormat="1">
+    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4005,7 +4125,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1">
+    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4036,7 +4156,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1">
+    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4067,7 +4187,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1">
+    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4098,7 +4218,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1">
+    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4129,7 +4249,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1">
+    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4160,7 +4280,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1">
+    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4191,7 +4311,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1">
+    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4222,7 +4342,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1">
+    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4253,7 +4373,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1">
+    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4284,7 +4404,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4315,7 +4435,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1">
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4346,7 +4466,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1">
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4377,7 +4497,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1">
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4408,7 +4528,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1">
+    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4439,7 +4559,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1">
+    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4470,7 +4590,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1">
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4501,7 +4621,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1">
+    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4532,7 +4652,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1">
+    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4563,7 +4683,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1">
+    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4594,7 +4714,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1">
+    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4625,7 +4745,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1">
+    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4656,7 +4776,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1">
+    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4687,7 +4807,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1">
+    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4718,7 +4838,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1">
+    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4749,7 +4869,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1">
+    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4780,7 +4900,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1">
+    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4811,7 +4931,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1">
+    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4842,7 +4962,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1">
+    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4873,7 +4993,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1">
+    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4904,7 +5024,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1">
+    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4935,7 +5055,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1">
+    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4966,7 +5086,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1">
+    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4997,7 +5117,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1">
+    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5028,7 +5148,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1">
+    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5059,7 +5179,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1">
+    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5090,7 +5210,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1">
+    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5121,7 +5241,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1">
+    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5152,7 +5272,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1">
+    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5183,7 +5303,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1">
+    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5214,7 +5334,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1">
+    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5245,7 +5365,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1">
+    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5276,7 +5396,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1">
+    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5307,7 +5427,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1">
+    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5338,7 +5458,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1">
+    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5369,7 +5489,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1">
+    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5400,7 +5520,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1">
+    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5431,7 +5551,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1">
+    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5462,7 +5582,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1">
+    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5493,7 +5613,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1">
+    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5524,7 +5644,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1">
+    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5555,7 +5675,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1">
+    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5586,7 +5706,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1">
+    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5617,7 +5737,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1">
+    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A101" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5648,7 +5768,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1">
+    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5679,7 +5799,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1">
+    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5710,7 +5830,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1">
+    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5741,7 +5861,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1">
+    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5772,7 +5892,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1">
+    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5803,7 +5923,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1">
+    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5834,7 +5954,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1">
+    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5866,7 +5986,7 @@
       <c r="K108" s="65"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="77H5Iqzv9dZcGmmBaf69JMJb19F7NL/TII5UwBSFOuUaqVrFbpC0VyStjTSM9GXqoLW1eBJcnDtnuP0mFWowpA==" saltValue="GBL6OckecvWR/Pgb/M/1sg==" spinCount="100000" sheet="1" scenarios="1" formatColumns="0" formatRows="0" selectLockedCells="1"/>
+  <sheetProtection formatColumns="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -5907,11 +6027,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5924,7 +6039,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="72.1640625" style="22" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="22"/>
@@ -5935,7 +6050,7 @@
     <col min="12" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>38</v>
       </c>
@@ -5945,7 +6060,7 @@
       <c r="E1" s="94"/>
       <c r="F1" s="95"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
@@ -5957,7 +6072,7 @@
       <c r="E2" s="98"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="60">
+    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
@@ -5981,7 +6096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6009,7 +6124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="76" thickBot="1">
+    <row r="5" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6036,7 +6151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31" thickBot="1">
+    <row r="6" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6058,7 +6173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="46" thickBot="1">
+    <row r="7" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6085,7 +6200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45">
+    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6104,7 +6219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45">
+    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6123,7 +6238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="31" thickBot="1">
+    <row r="10" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6142,7 +6257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6153,7 +6268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" thickBot="1">
+    <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6164,7 +6279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="93" t="s">
         <v>41</v>
       </c>
@@ -6183,7 +6298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" thickBot="1">
+    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6200,7 +6315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -6218,7 +6333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67" customHeight="1">
+    <row r="16" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6242,7 +6357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6263,7 +6378,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="76" thickBot="1">
+    <row r="18" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6284,7 +6399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6303,7 +6418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="61" thickBot="1">
+    <row r="20" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6325,7 +6440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6342,122 +6457,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6646,11 +6761,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6663,7 +6773,7 @@
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="22" customWidth="1"/>
@@ -6678,7 +6788,7 @@
     <col min="11" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="108" t="s">
         <v>56</v>
       </c>
@@ -6705,7 +6815,7 @@
       </c>
       <c r="I1" s="107"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -6720,7 +6830,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -6745,7 +6855,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -6774,7 +6884,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -6803,7 +6913,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -6832,7 +6942,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -6857,7 +6967,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -6886,7 +6996,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -6915,7 +7025,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -6944,7 +7054,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -6969,7 +7079,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -6998,7 +7108,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7027,7 +7137,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.75" customHeight="1">
+    <row r="14" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7050,7 +7160,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.75" customHeight="1">
+    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="75" t="s">
         <v>96</v>
       </c>
@@ -7076,7 +7186,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.75" customHeight="1">
+    <row r="16" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7104,7 +7214,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.75" customHeight="1">
+    <row r="17" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7132,7 +7242,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.75" customHeight="1">
+    <row r="18" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7158,7 +7268,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.75" customHeight="1">
+    <row r="19" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7182,7 +7292,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.75" customHeight="1">
+    <row r="20" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7206,7 +7316,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.75" customHeight="1">
+    <row r="21" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7230,7 +7340,7 @@
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.75" customHeight="1">
+    <row r="22" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7254,7 +7364,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.75" customHeight="1">
+    <row r="23" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7283,7 +7393,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.75" customHeight="1">
+    <row r="24" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7306,7 +7416,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
-    <row r="25" spans="1:10" ht="14.75" customHeight="1">
+    <row r="25" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7330,7 +7440,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.75" customHeight="1">
+    <row r="26" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7359,7 +7469,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.75" customHeight="1">
+    <row r="27" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7383,7 +7493,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.75" customHeight="1">
+    <row r="28" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7407,7 +7517,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.75" customHeight="1">
+    <row r="29" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7436,7 +7546,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.75" customHeight="1">
+    <row r="30" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7459,7 +7569,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.75" customHeight="1">
+    <row r="31" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7476,7 +7586,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.75" customHeight="1">
+    <row r="32" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7491,7 +7601,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.75" customHeight="1">
+    <row r="33" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7512,7 +7622,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.75" customHeight="1">
+    <row r="34" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7529,7 +7639,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.75" customHeight="1">
+    <row r="35" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7558,7 +7668,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.75" customHeight="1">
+    <row r="36" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7587,7 +7697,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.75" customHeight="1">
+    <row r="37" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7610,7 +7720,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.75" customHeight="1">
+    <row r="38" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7633,13 +7743,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7653,7 +7763,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -7667,7 +7777,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -7681,7 +7791,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7695,7 +7805,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -7709,7 +7819,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="45">
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>
@@ -7736,10 +7846,5 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>